<commit_message>
completed test for specimen collected by dso
</commit_message>
<xml_diff>
--- a/forms/app/specimen_details.xlsx
+++ b/forms/app/specimen_details.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -405,6 +405,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Sample Taken on ${</t>
     </r>
@@ -414,6 +415,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">follow_up_date</t>
     </r>
@@ -423,6 +425,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">}</t>
     </r>
@@ -440,6 +443,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Specimen Collected ${</t>
     </r>
@@ -449,6 +453,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">specimen_type</t>
     </r>
@@ -458,6 +463,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">}</t>
     </r>
@@ -484,6 +490,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">specimen_type</t>
     </r>
@@ -525,6 +532,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">result</t>
     </r>
@@ -560,6 +568,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">result</t>
     </r>
@@ -688,7 +697,7 @@
     <t xml:space="preserve">Laboratory Report</t>
   </si>
   <si>
-    <t xml:space="preserve">specimen_form</t>
+    <t xml:space="preserve">specimen_details</t>
   </si>
   <si>
     <t xml:space="preserve">pages</t>
@@ -708,7 +717,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd\-mm\-yyyy\ hh\-mm\-ss"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -769,6 +778,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -782,18 +792,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -809,13 +815,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
@@ -986,7 +985,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1087,35 +1086,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1123,15 +1118,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1139,10 +1134,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1151,67 +1142,63 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1294,11 +1281,11 @@
   </sheetPr>
   <dimension ref="A1:AJ96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B60" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B37" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C74" activeCellId="0" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.55"/>
@@ -3595,7 +3582,6 @@
       <c r="C75" s="26"/>
       <c r="D75" s="26"/>
       <c r="E75" s="26"/>
-      <c r="F75" s="27"/>
       <c r="G75" s="26"/>
       <c r="H75" s="26"/>
       <c r="I75" s="26"/>
@@ -3787,39 +3773,6 @@
       <c r="AD80" s="26"/>
       <c r="AE80" s="26"/>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="27"/>
-      <c r="B81" s="27"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
-      <c r="G81" s="27"/>
-      <c r="H81" s="27"/>
-      <c r="I81" s="27"/>
-      <c r="J81" s="27"/>
-      <c r="K81" s="27"/>
-      <c r="L81" s="27"/>
-      <c r="M81" s="27"/>
-      <c r="N81" s="27"/>
-      <c r="O81" s="27"/>
-      <c r="P81" s="27"/>
-      <c r="Q81" s="27"/>
-      <c r="R81" s="27"/>
-      <c r="S81" s="27"/>
-      <c r="T81" s="27"/>
-      <c r="U81" s="27"/>
-      <c r="V81" s="27"/>
-      <c r="W81" s="27"/>
-      <c r="X81" s="27"/>
-      <c r="Y81" s="27"/>
-      <c r="Z81" s="27"/>
-      <c r="AA81" s="27"/>
-      <c r="AB81" s="27"/>
-      <c r="AC81" s="27"/>
-      <c r="AD81" s="27"/>
-      <c r="AE81" s="27"/>
-    </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="26"/>
       <c r="B82" s="26"/>
@@ -3854,445 +3807,399 @@
       <c r="AE82" s="26"/>
     </row>
     <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="28"/>
-      <c r="B83" s="29"/>
-      <c r="C83" s="30"/>
-      <c r="D83" s="28"/>
-      <c r="E83" s="31"/>
-      <c r="F83" s="27"/>
-      <c r="G83" s="28"/>
-      <c r="H83" s="31"/>
-      <c r="I83" s="31"/>
-      <c r="J83" s="31"/>
-      <c r="K83" s="28"/>
-      <c r="L83" s="31"/>
-      <c r="M83" s="32"/>
-      <c r="N83" s="31"/>
-      <c r="O83" s="31"/>
-      <c r="P83" s="33"/>
-      <c r="Q83" s="33"/>
-      <c r="R83" s="33"/>
-      <c r="S83" s="33"/>
-      <c r="T83" s="33"/>
-      <c r="U83" s="33"/>
-      <c r="V83" s="33"/>
-      <c r="W83" s="33"/>
-      <c r="X83" s="33"/>
-      <c r="Y83" s="33"/>
-      <c r="Z83" s="33"/>
-      <c r="AA83" s="27"/>
-      <c r="AB83" s="27"/>
-      <c r="AC83" s="27"/>
-      <c r="AD83" s="27"/>
-      <c r="AE83" s="27"/>
+      <c r="A83" s="27"/>
+      <c r="B83" s="28"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="27"/>
+      <c r="E83" s="30"/>
+      <c r="G83" s="27"/>
+      <c r="H83" s="30"/>
+      <c r="I83" s="30"/>
+      <c r="J83" s="30"/>
+      <c r="K83" s="27"/>
+      <c r="L83" s="30"/>
+      <c r="M83" s="31"/>
+      <c r="N83" s="30"/>
+      <c r="O83" s="30"/>
+      <c r="P83" s="32"/>
+      <c r="Q83" s="32"/>
+      <c r="R83" s="32"/>
+      <c r="S83" s="32"/>
+      <c r="T83" s="32"/>
+      <c r="U83" s="32"/>
+      <c r="V83" s="32"/>
+      <c r="W83" s="32"/>
+      <c r="X83" s="32"/>
+      <c r="Y83" s="32"/>
+      <c r="Z83" s="32"/>
     </row>
     <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="30"/>
-      <c r="B84" s="30"/>
-      <c r="C84" s="30"/>
-      <c r="D84" s="28"/>
-      <c r="E84" s="30"/>
-      <c r="F84" s="30"/>
-      <c r="G84" s="30"/>
-      <c r="H84" s="30"/>
-      <c r="I84" s="30"/>
-      <c r="J84" s="30"/>
-      <c r="K84" s="28"/>
-      <c r="L84" s="30"/>
-      <c r="M84" s="30"/>
-      <c r="N84" s="30"/>
-      <c r="O84" s="30"/>
-      <c r="P84" s="30"/>
-      <c r="Q84" s="30"/>
-      <c r="R84" s="30"/>
-      <c r="S84" s="30"/>
-      <c r="T84" s="30"/>
-      <c r="U84" s="30"/>
-      <c r="V84" s="30"/>
-      <c r="W84" s="30"/>
-      <c r="X84" s="30"/>
-      <c r="Y84" s="30"/>
-      <c r="Z84" s="30"/>
-      <c r="AA84" s="27"/>
-      <c r="AB84" s="27"/>
-      <c r="AC84" s="27"/>
-      <c r="AD84" s="27"/>
-      <c r="AE84" s="27"/>
+      <c r="A84" s="29"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="29"/>
+      <c r="D84" s="27"/>
+      <c r="E84" s="29"/>
+      <c r="F84" s="29"/>
+      <c r="G84" s="29"/>
+      <c r="H84" s="29"/>
+      <c r="I84" s="29"/>
+      <c r="J84" s="29"/>
+      <c r="K84" s="27"/>
+      <c r="L84" s="29"/>
+      <c r="M84" s="29"/>
+      <c r="N84" s="29"/>
+      <c r="O84" s="29"/>
+      <c r="P84" s="29"/>
+      <c r="Q84" s="29"/>
+      <c r="R84" s="29"/>
+      <c r="S84" s="29"/>
+      <c r="T84" s="29"/>
+      <c r="U84" s="29"/>
+      <c r="V84" s="29"/>
+      <c r="W84" s="29"/>
+      <c r="X84" s="29"/>
+      <c r="Y84" s="29"/>
+      <c r="Z84" s="29"/>
     </row>
     <row r="85" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="30"/>
-      <c r="B85" s="30"/>
-      <c r="C85" s="30"/>
-      <c r="D85" s="28"/>
-      <c r="E85" s="30"/>
-      <c r="F85" s="34"/>
-      <c r="G85" s="29"/>
-      <c r="H85" s="30"/>
-      <c r="I85" s="30"/>
-      <c r="J85" s="30"/>
-      <c r="K85" s="28"/>
-      <c r="L85" s="30"/>
-      <c r="M85" s="30"/>
-      <c r="N85" s="30"/>
-      <c r="O85" s="30"/>
-      <c r="P85" s="30"/>
-      <c r="Q85" s="30"/>
-      <c r="R85" s="30"/>
-      <c r="S85" s="30"/>
-      <c r="T85" s="30"/>
-      <c r="U85" s="30"/>
-      <c r="V85" s="30"/>
-      <c r="W85" s="30"/>
-      <c r="X85" s="30"/>
-      <c r="Y85" s="30"/>
-      <c r="Z85" s="30"/>
-      <c r="AA85" s="27"/>
-      <c r="AB85" s="27"/>
-      <c r="AC85" s="27"/>
-      <c r="AD85" s="27"/>
-      <c r="AE85" s="27"/>
+      <c r="A85" s="29"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="27"/>
+      <c r="E85" s="29"/>
+      <c r="F85" s="33"/>
+      <c r="G85" s="28"/>
+      <c r="H85" s="29"/>
+      <c r="I85" s="29"/>
+      <c r="J85" s="29"/>
+      <c r="K85" s="27"/>
+      <c r="L85" s="29"/>
+      <c r="M85" s="29"/>
+      <c r="N85" s="29"/>
+      <c r="O85" s="29"/>
+      <c r="P85" s="29"/>
+      <c r="Q85" s="29"/>
+      <c r="R85" s="29"/>
+      <c r="S85" s="29"/>
+      <c r="T85" s="29"/>
+      <c r="U85" s="29"/>
+      <c r="V85" s="29"/>
+      <c r="W85" s="29"/>
+      <c r="X85" s="29"/>
+      <c r="Y85" s="29"/>
+      <c r="Z85" s="29"/>
     </row>
     <row r="86" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="30"/>
-      <c r="B86" s="30"/>
-      <c r="C86" s="30"/>
-      <c r="D86" s="28"/>
-      <c r="E86" s="30"/>
-      <c r="F86" s="34"/>
-      <c r="G86" s="30"/>
-      <c r="H86" s="30"/>
-      <c r="I86" s="30"/>
-      <c r="J86" s="30"/>
-      <c r="K86" s="28"/>
-      <c r="L86" s="30"/>
-      <c r="M86" s="30"/>
-      <c r="N86" s="30"/>
-      <c r="O86" s="30"/>
-      <c r="P86" s="30"/>
-      <c r="Q86" s="30"/>
-      <c r="R86" s="30"/>
-      <c r="S86" s="30"/>
-      <c r="T86" s="30"/>
-      <c r="U86" s="30"/>
-      <c r="V86" s="30"/>
-      <c r="W86" s="30"/>
-      <c r="X86" s="30"/>
-      <c r="Y86" s="30"/>
-      <c r="Z86" s="30"/>
-      <c r="AA86" s="27"/>
-      <c r="AB86" s="27"/>
-      <c r="AC86" s="27"/>
-      <c r="AD86" s="27"/>
-      <c r="AE86" s="27"/>
+      <c r="A86" s="29"/>
+      <c r="B86" s="29"/>
+      <c r="C86" s="29"/>
+      <c r="D86" s="27"/>
+      <c r="E86" s="29"/>
+      <c r="F86" s="33"/>
+      <c r="G86" s="29"/>
+      <c r="H86" s="29"/>
+      <c r="I86" s="29"/>
+      <c r="J86" s="29"/>
+      <c r="K86" s="27"/>
+      <c r="L86" s="29"/>
+      <c r="M86" s="29"/>
+      <c r="N86" s="29"/>
+      <c r="O86" s="29"/>
+      <c r="P86" s="29"/>
+      <c r="Q86" s="29"/>
+      <c r="R86" s="29"/>
+      <c r="S86" s="29"/>
+      <c r="T86" s="29"/>
+      <c r="U86" s="29"/>
+      <c r="V86" s="29"/>
+      <c r="W86" s="29"/>
+      <c r="X86" s="29"/>
+      <c r="Y86" s="29"/>
+      <c r="Z86" s="29"/>
     </row>
     <row r="87" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="30"/>
-      <c r="B87" s="30"/>
-      <c r="C87" s="30"/>
-      <c r="D87" s="28"/>
-      <c r="E87" s="30"/>
-      <c r="F87" s="34"/>
-      <c r="G87" s="29"/>
-      <c r="H87" s="30"/>
-      <c r="I87" s="30"/>
-      <c r="J87" s="30"/>
-      <c r="K87" s="28"/>
-      <c r="L87" s="30"/>
-      <c r="M87" s="30"/>
-      <c r="N87" s="30"/>
-      <c r="O87" s="30"/>
-      <c r="P87" s="30"/>
-      <c r="Q87" s="30"/>
-      <c r="R87" s="30"/>
-      <c r="S87" s="30"/>
-      <c r="T87" s="30"/>
-      <c r="U87" s="30"/>
-      <c r="V87" s="30"/>
-      <c r="W87" s="30"/>
-      <c r="X87" s="30"/>
-      <c r="Y87" s="30"/>
-      <c r="Z87" s="30"/>
-      <c r="AA87" s="27"/>
-      <c r="AB87" s="27"/>
-      <c r="AC87" s="27"/>
-      <c r="AD87" s="27"/>
-      <c r="AE87" s="27"/>
+      <c r="A87" s="29"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="29"/>
+      <c r="D87" s="27"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="33"/>
+      <c r="G87" s="28"/>
+      <c r="H87" s="29"/>
+      <c r="I87" s="29"/>
+      <c r="J87" s="29"/>
+      <c r="K87" s="27"/>
+      <c r="L87" s="29"/>
+      <c r="M87" s="29"/>
+      <c r="N87" s="29"/>
+      <c r="O87" s="29"/>
+      <c r="P87" s="29"/>
+      <c r="Q87" s="29"/>
+      <c r="R87" s="29"/>
+      <c r="S87" s="29"/>
+      <c r="T87" s="29"/>
+      <c r="U87" s="29"/>
+      <c r="V87" s="29"/>
+      <c r="W87" s="29"/>
+      <c r="X87" s="29"/>
+      <c r="Y87" s="29"/>
+      <c r="Z87" s="29"/>
     </row>
     <row r="88" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="30"/>
-      <c r="B88" s="30"/>
-      <c r="C88" s="30"/>
-      <c r="D88" s="28"/>
-      <c r="E88" s="30"/>
-      <c r="F88" s="34"/>
-      <c r="G88" s="29"/>
-      <c r="H88" s="30"/>
-      <c r="I88" s="30"/>
-      <c r="J88" s="30"/>
-      <c r="K88" s="28"/>
-      <c r="L88" s="30"/>
-      <c r="M88" s="30"/>
-      <c r="N88" s="30"/>
-      <c r="O88" s="30"/>
-      <c r="P88" s="30"/>
-      <c r="Q88" s="30"/>
-      <c r="R88" s="30"/>
-      <c r="S88" s="30"/>
-      <c r="T88" s="30"/>
-      <c r="U88" s="30"/>
-      <c r="V88" s="30"/>
-      <c r="W88" s="30"/>
-      <c r="X88" s="30"/>
-      <c r="Y88" s="30"/>
-      <c r="Z88" s="30"/>
-      <c r="AA88" s="27"/>
-      <c r="AB88" s="27"/>
-      <c r="AC88" s="27"/>
-      <c r="AD88" s="27"/>
-      <c r="AE88" s="27"/>
+      <c r="A88" s="29"/>
+      <c r="B88" s="29"/>
+      <c r="C88" s="29"/>
+      <c r="D88" s="27"/>
+      <c r="E88" s="29"/>
+      <c r="F88" s="33"/>
+      <c r="G88" s="28"/>
+      <c r="H88" s="29"/>
+      <c r="I88" s="29"/>
+      <c r="J88" s="29"/>
+      <c r="K88" s="27"/>
+      <c r="L88" s="29"/>
+      <c r="M88" s="29"/>
+      <c r="N88" s="29"/>
+      <c r="O88" s="29"/>
+      <c r="P88" s="29"/>
+      <c r="Q88" s="29"/>
+      <c r="R88" s="29"/>
+      <c r="S88" s="29"/>
+      <c r="T88" s="29"/>
+      <c r="U88" s="29"/>
+      <c r="V88" s="29"/>
+      <c r="W88" s="29"/>
+      <c r="X88" s="29"/>
+      <c r="Y88" s="29"/>
+      <c r="Z88" s="29"/>
     </row>
     <row r="89" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="30"/>
-      <c r="B89" s="29"/>
-      <c r="C89" s="30"/>
-      <c r="D89" s="29"/>
-      <c r="E89" s="29"/>
-      <c r="F89" s="31"/>
-      <c r="G89" s="29"/>
-      <c r="H89" s="30"/>
-      <c r="I89" s="30"/>
-      <c r="J89" s="30"/>
-      <c r="K89" s="28"/>
-      <c r="L89" s="30"/>
-      <c r="M89" s="30"/>
-      <c r="N89" s="30"/>
-      <c r="O89" s="30"/>
-      <c r="P89" s="30"/>
-      <c r="Q89" s="30"/>
-      <c r="R89" s="30"/>
-      <c r="S89" s="30"/>
-      <c r="T89" s="30"/>
-      <c r="U89" s="30"/>
-      <c r="V89" s="30"/>
-      <c r="W89" s="30"/>
-      <c r="X89" s="30"/>
-      <c r="Y89" s="30"/>
-      <c r="Z89" s="30"/>
-      <c r="AA89" s="27"/>
-      <c r="AB89" s="27"/>
-      <c r="AC89" s="27"/>
-      <c r="AD89" s="27"/>
-      <c r="AE89" s="27"/>
+      <c r="A89" s="29"/>
+      <c r="B89" s="28"/>
+      <c r="C89" s="29"/>
+      <c r="D89" s="28"/>
+      <c r="E89" s="28"/>
+      <c r="F89" s="30"/>
+      <c r="G89" s="28"/>
+      <c r="H89" s="29"/>
+      <c r="I89" s="29"/>
+      <c r="J89" s="29"/>
+      <c r="K89" s="27"/>
+      <c r="L89" s="29"/>
+      <c r="M89" s="29"/>
+      <c r="N89" s="29"/>
+      <c r="O89" s="29"/>
+      <c r="P89" s="29"/>
+      <c r="Q89" s="29"/>
+      <c r="R89" s="29"/>
+      <c r="S89" s="29"/>
+      <c r="T89" s="29"/>
+      <c r="U89" s="29"/>
+      <c r="V89" s="29"/>
+      <c r="W89" s="29"/>
+      <c r="X89" s="29"/>
+      <c r="Y89" s="29"/>
+      <c r="Z89" s="29"/>
     </row>
     <row r="90" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="30"/>
-      <c r="B90" s="29"/>
-      <c r="C90" s="30"/>
-      <c r="D90" s="29"/>
-      <c r="E90" s="29"/>
-      <c r="F90" s="31"/>
-      <c r="G90" s="29"/>
-      <c r="H90" s="30"/>
-      <c r="I90" s="30"/>
-      <c r="J90" s="30"/>
-      <c r="K90" s="28"/>
-      <c r="L90" s="30"/>
-      <c r="M90" s="30"/>
-      <c r="N90" s="30"/>
-      <c r="O90" s="30"/>
-      <c r="P90" s="30"/>
-      <c r="Q90" s="30"/>
-      <c r="R90" s="30"/>
-      <c r="S90" s="30"/>
-      <c r="T90" s="30"/>
-      <c r="U90" s="30"/>
-      <c r="V90" s="30"/>
-      <c r="W90" s="30"/>
-      <c r="X90" s="30"/>
-      <c r="Y90" s="30"/>
-      <c r="Z90" s="30"/>
-      <c r="AA90" s="27"/>
-      <c r="AB90" s="27"/>
-      <c r="AC90" s="27"/>
-      <c r="AD90" s="27"/>
-      <c r="AE90" s="27"/>
+      <c r="A90" s="29"/>
+      <c r="B90" s="28"/>
+      <c r="C90" s="29"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="28"/>
+      <c r="F90" s="30"/>
+      <c r="G90" s="28"/>
+      <c r="H90" s="29"/>
+      <c r="I90" s="29"/>
+      <c r="J90" s="29"/>
+      <c r="K90" s="27"/>
+      <c r="L90" s="29"/>
+      <c r="M90" s="29"/>
+      <c r="N90" s="29"/>
+      <c r="O90" s="29"/>
+      <c r="P90" s="29"/>
+      <c r="Q90" s="29"/>
+      <c r="R90" s="29"/>
+      <c r="S90" s="29"/>
+      <c r="T90" s="29"/>
+      <c r="U90" s="29"/>
+      <c r="V90" s="29"/>
+      <c r="W90" s="29"/>
+      <c r="X90" s="29"/>
+      <c r="Y90" s="29"/>
+      <c r="Z90" s="29"/>
     </row>
     <row r="91" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="30"/>
-      <c r="B91" s="29"/>
-      <c r="C91" s="30"/>
-      <c r="D91" s="29"/>
-      <c r="E91" s="29"/>
-      <c r="F91" s="31"/>
-      <c r="G91" s="29"/>
-      <c r="H91" s="30"/>
-      <c r="I91" s="30"/>
-      <c r="J91" s="30"/>
-      <c r="K91" s="28"/>
-      <c r="L91" s="30"/>
-      <c r="M91" s="30"/>
-      <c r="N91" s="30"/>
-      <c r="O91" s="30"/>
-      <c r="P91" s="30"/>
-      <c r="Q91" s="30"/>
-      <c r="R91" s="30"/>
-      <c r="S91" s="30"/>
-      <c r="T91" s="30"/>
-      <c r="U91" s="30"/>
-      <c r="V91" s="30"/>
-      <c r="W91" s="30"/>
-      <c r="X91" s="30"/>
-      <c r="Y91" s="30"/>
-      <c r="Z91" s="30"/>
-      <c r="AA91" s="27"/>
-      <c r="AB91" s="27"/>
-      <c r="AC91" s="27"/>
-      <c r="AD91" s="27"/>
-      <c r="AE91" s="27"/>
+      <c r="A91" s="29"/>
+      <c r="B91" s="28"/>
+      <c r="C91" s="29"/>
+      <c r="D91" s="28"/>
+      <c r="E91" s="28"/>
+      <c r="F91" s="30"/>
+      <c r="G91" s="28"/>
+      <c r="H91" s="29"/>
+      <c r="I91" s="29"/>
+      <c r="J91" s="29"/>
+      <c r="K91" s="27"/>
+      <c r="L91" s="29"/>
+      <c r="M91" s="29"/>
+      <c r="N91" s="29"/>
+      <c r="O91" s="29"/>
+      <c r="P91" s="29"/>
+      <c r="Q91" s="29"/>
+      <c r="R91" s="29"/>
+      <c r="S91" s="29"/>
+      <c r="T91" s="29"/>
+      <c r="U91" s="29"/>
+      <c r="V91" s="29"/>
+      <c r="W91" s="29"/>
+      <c r="X91" s="29"/>
+      <c r="Y91" s="29"/>
+      <c r="Z91" s="29"/>
     </row>
     <row r="92" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="30"/>
-      <c r="B92" s="29"/>
-      <c r="C92" s="30"/>
-      <c r="D92" s="29"/>
-      <c r="E92" s="29"/>
-      <c r="F92" s="31"/>
-      <c r="G92" s="29"/>
-      <c r="H92" s="30"/>
-      <c r="I92" s="35"/>
-      <c r="J92" s="35"/>
-      <c r="K92" s="36"/>
-      <c r="L92" s="35"/>
-      <c r="M92" s="35"/>
-      <c r="N92" s="35"/>
-      <c r="O92" s="35"/>
-      <c r="P92" s="35"/>
-      <c r="Q92" s="35"/>
-      <c r="R92" s="35"/>
-      <c r="S92" s="35"/>
-      <c r="T92" s="35"/>
-      <c r="U92" s="35"/>
-      <c r="V92" s="35"/>
-      <c r="W92" s="35"/>
-      <c r="X92" s="35"/>
-      <c r="Y92" s="35"/>
-      <c r="Z92" s="35"/>
-      <c r="AA92" s="37"/>
-      <c r="AB92" s="37"/>
+      <c r="A92" s="29"/>
+      <c r="B92" s="28"/>
+      <c r="C92" s="29"/>
+      <c r="D92" s="28"/>
+      <c r="E92" s="28"/>
+      <c r="F92" s="30"/>
+      <c r="G92" s="28"/>
+      <c r="H92" s="29"/>
+      <c r="I92" s="34"/>
+      <c r="J92" s="34"/>
+      <c r="K92" s="35"/>
+      <c r="L92" s="34"/>
+      <c r="M92" s="34"/>
+      <c r="N92" s="34"/>
+      <c r="O92" s="34"/>
+      <c r="P92" s="34"/>
+      <c r="Q92" s="34"/>
+      <c r="R92" s="34"/>
+      <c r="S92" s="34"/>
+      <c r="T92" s="34"/>
+      <c r="U92" s="34"/>
+      <c r="V92" s="34"/>
+      <c r="W92" s="34"/>
+      <c r="X92" s="34"/>
+      <c r="Y92" s="34"/>
+      <c r="Z92" s="34"/>
+      <c r="AA92" s="36"/>
+      <c r="AB92" s="36"/>
     </row>
     <row r="93" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="30"/>
-      <c r="B93" s="29"/>
-      <c r="C93" s="30"/>
-      <c r="D93" s="29"/>
-      <c r="E93" s="29"/>
-      <c r="F93" s="31"/>
-      <c r="G93" s="29"/>
-      <c r="H93" s="30"/>
-      <c r="I93" s="35"/>
-      <c r="J93" s="35"/>
-      <c r="K93" s="36"/>
-      <c r="L93" s="35"/>
-      <c r="M93" s="35"/>
-      <c r="N93" s="35"/>
-      <c r="O93" s="35"/>
-      <c r="P93" s="35"/>
-      <c r="Q93" s="35"/>
-      <c r="R93" s="35"/>
-      <c r="S93" s="35"/>
-      <c r="T93" s="35"/>
-      <c r="U93" s="35"/>
-      <c r="V93" s="35"/>
-      <c r="W93" s="35"/>
-      <c r="X93" s="35"/>
-      <c r="Y93" s="35"/>
-      <c r="Z93" s="35"/>
-      <c r="AA93" s="37"/>
-      <c r="AB93" s="37"/>
+      <c r="A93" s="29"/>
+      <c r="B93" s="28"/>
+      <c r="C93" s="29"/>
+      <c r="D93" s="28"/>
+      <c r="E93" s="28"/>
+      <c r="F93" s="30"/>
+      <c r="G93" s="28"/>
+      <c r="H93" s="29"/>
+      <c r="I93" s="34"/>
+      <c r="J93" s="34"/>
+      <c r="K93" s="35"/>
+      <c r="L93" s="34"/>
+      <c r="M93" s="34"/>
+      <c r="N93" s="34"/>
+      <c r="O93" s="34"/>
+      <c r="P93" s="34"/>
+      <c r="Q93" s="34"/>
+      <c r="R93" s="34"/>
+      <c r="S93" s="34"/>
+      <c r="T93" s="34"/>
+      <c r="U93" s="34"/>
+      <c r="V93" s="34"/>
+      <c r="W93" s="34"/>
+      <c r="X93" s="34"/>
+      <c r="Y93" s="34"/>
+      <c r="Z93" s="34"/>
+      <c r="AA93" s="36"/>
+      <c r="AB93" s="36"/>
     </row>
     <row r="94" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="30"/>
-      <c r="B94" s="29"/>
-      <c r="C94" s="30"/>
-      <c r="D94" s="29"/>
-      <c r="E94" s="29"/>
-      <c r="F94" s="31"/>
-      <c r="G94" s="29"/>
-      <c r="H94" s="30"/>
-      <c r="I94" s="35"/>
-      <c r="J94" s="35"/>
-      <c r="K94" s="36"/>
-      <c r="L94" s="35"/>
-      <c r="M94" s="35"/>
-      <c r="N94" s="35"/>
-      <c r="O94" s="35"/>
-      <c r="P94" s="35"/>
-      <c r="Q94" s="35"/>
-      <c r="R94" s="35"/>
-      <c r="S94" s="35"/>
-      <c r="T94" s="35"/>
-      <c r="U94" s="35"/>
-      <c r="V94" s="35"/>
-      <c r="W94" s="35"/>
-      <c r="X94" s="35"/>
-      <c r="Y94" s="35"/>
-      <c r="Z94" s="35"/>
-      <c r="AA94" s="37"/>
-      <c r="AB94" s="37"/>
+      <c r="A94" s="29"/>
+      <c r="B94" s="28"/>
+      <c r="C94" s="29"/>
+      <c r="D94" s="28"/>
+      <c r="E94" s="28"/>
+      <c r="F94" s="30"/>
+      <c r="G94" s="28"/>
+      <c r="H94" s="29"/>
+      <c r="I94" s="34"/>
+      <c r="J94" s="34"/>
+      <c r="K94" s="35"/>
+      <c r="L94" s="34"/>
+      <c r="M94" s="34"/>
+      <c r="N94" s="34"/>
+      <c r="O94" s="34"/>
+      <c r="P94" s="34"/>
+      <c r="Q94" s="34"/>
+      <c r="R94" s="34"/>
+      <c r="S94" s="34"/>
+      <c r="T94" s="34"/>
+      <c r="U94" s="34"/>
+      <c r="V94" s="34"/>
+      <c r="W94" s="34"/>
+      <c r="X94" s="34"/>
+      <c r="Y94" s="34"/>
+      <c r="Z94" s="34"/>
+      <c r="AA94" s="36"/>
+      <c r="AB94" s="36"/>
     </row>
     <row r="95" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="30"/>
-      <c r="B95" s="29"/>
-      <c r="C95" s="30"/>
-      <c r="D95" s="29"/>
-      <c r="E95" s="29"/>
-      <c r="F95" s="31"/>
-      <c r="G95" s="29"/>
-      <c r="H95" s="30"/>
-      <c r="I95" s="35"/>
-      <c r="J95" s="35"/>
-      <c r="K95" s="36"/>
-      <c r="L95" s="35"/>
-      <c r="M95" s="35"/>
-      <c r="N95" s="35"/>
-      <c r="O95" s="35"/>
-      <c r="P95" s="35"/>
-      <c r="Q95" s="35"/>
-      <c r="R95" s="35"/>
-      <c r="S95" s="35"/>
-      <c r="T95" s="35"/>
-      <c r="U95" s="35"/>
-      <c r="V95" s="35"/>
-      <c r="W95" s="35"/>
-      <c r="X95" s="35"/>
-      <c r="Y95" s="35"/>
-      <c r="Z95" s="35"/>
-      <c r="AA95" s="37"/>
-      <c r="AB95" s="37"/>
+      <c r="A95" s="29"/>
+      <c r="B95" s="28"/>
+      <c r="C95" s="29"/>
+      <c r="D95" s="28"/>
+      <c r="E95" s="28"/>
+      <c r="F95" s="30"/>
+      <c r="G95" s="28"/>
+      <c r="H95" s="29"/>
+      <c r="I95" s="34"/>
+      <c r="J95" s="34"/>
+      <c r="K95" s="35"/>
+      <c r="L95" s="34"/>
+      <c r="M95" s="34"/>
+      <c r="N95" s="34"/>
+      <c r="O95" s="34"/>
+      <c r="P95" s="34"/>
+      <c r="Q95" s="34"/>
+      <c r="R95" s="34"/>
+      <c r="S95" s="34"/>
+      <c r="T95" s="34"/>
+      <c r="U95" s="34"/>
+      <c r="V95" s="34"/>
+      <c r="W95" s="34"/>
+      <c r="X95" s="34"/>
+      <c r="Y95" s="34"/>
+      <c r="Z95" s="34"/>
+      <c r="AA95" s="36"/>
+      <c r="AB95" s="36"/>
     </row>
     <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="38"/>
-      <c r="H96" s="39"/>
-      <c r="I96" s="39"/>
-      <c r="J96" s="35"/>
-      <c r="K96" s="36"/>
-      <c r="L96" s="39"/>
-      <c r="M96" s="39"/>
-      <c r="N96" s="39"/>
-      <c r="O96" s="39"/>
-      <c r="P96" s="39"/>
-      <c r="Q96" s="39"/>
-      <c r="R96" s="39"/>
-      <c r="S96" s="39"/>
-      <c r="T96" s="39"/>
-      <c r="U96" s="39"/>
-      <c r="V96" s="39"/>
-      <c r="W96" s="39"/>
-      <c r="X96" s="39"/>
-      <c r="Y96" s="39"/>
-      <c r="Z96" s="39"/>
-      <c r="AA96" s="37"/>
-      <c r="AB96" s="37"/>
+      <c r="A96" s="28"/>
+      <c r="H96" s="37"/>
+      <c r="I96" s="37"/>
+      <c r="J96" s="34"/>
+      <c r="K96" s="35"/>
+      <c r="L96" s="37"/>
+      <c r="M96" s="37"/>
+      <c r="N96" s="37"/>
+      <c r="O96" s="37"/>
+      <c r="P96" s="37"/>
+      <c r="Q96" s="37"/>
+      <c r="R96" s="37"/>
+      <c r="S96" s="37"/>
+      <c r="T96" s="37"/>
+      <c r="U96" s="37"/>
+      <c r="V96" s="37"/>
+      <c r="W96" s="37"/>
+      <c r="X96" s="37"/>
+      <c r="Y96" s="37"/>
+      <c r="Z96" s="37"/>
+      <c r="AA96" s="36"/>
+      <c r="AB96" s="36"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -4330,191 +4237,191 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="40" width="28.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="40" width="45.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="38" width="28.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="38" width="45.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="49"/>
-      <c r="U1" s="49"/>
-      <c r="V1" s="49"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="47" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="51"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="47" t="s">
         <v>157</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="47" t="s">
         <v>159</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="48" t="s">
         <v>160</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="51"/>
-      <c r="U3" s="51"/>
-      <c r="V3" s="51"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="49"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="51"/>
-      <c r="U4" s="51"/>
-      <c r="V4" s="51"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="49"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="38" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="38" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="38" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="38" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="38" t="s">
         <v>169</v>
       </c>
     </row>
@@ -4587,57 +4494,57 @@
   </sheetPr>
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="50" t="s">
         <v>176</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
-      <c r="X1" s="41"/>
-      <c r="Y1" s="41"/>
-      <c r="Z1" s="41"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
@@ -4646,39 +4553,39 @@
       <c r="B2" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="C2" s="54" t="n">
+      <c r="C2" s="51" t="n">
         <f aca="true">NOW()</f>
-        <v>45316.8564730556</v>
-      </c>
-      <c r="D2" s="55" t="s">
+        <v>45328.9949586834</v>
+      </c>
+      <c r="D2" s="52" t="s">
         <v>179</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="52" t="s">
         <v>180</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="56" t="s">
+      <c r="F2" s="47"/>
+      <c r="G2" s="53" t="s">
         <v>181</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="49"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="47"/>
+      <c r="Z2" s="47"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>